<commit_message>
improved background and sizes
</commit_message>
<xml_diff>
--- a/antifibrotic_trials.xlsx
+++ b/antifibrotic_trials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterhiggins/Documents/RCode/antifibrotics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07349116-6D4E-9143-916E-6E0DC228CD12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA1DC0D-148D-9940-8E84-D61CD863FDD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="10200" windowWidth="21540" windowHeight="17440" xr2:uid="{64EA9187-3F1F-C745-9F47-CCBACCB200F3}"/>
   </bookViews>
@@ -80,9 +80,6 @@
     <t>Atorvastatin</t>
   </si>
   <si>
-    <t>HMGCoA</t>
-  </si>
-  <si>
     <t>Heart</t>
   </si>
   <si>
@@ -92,18 +89,12 @@
     <t>Candesartan</t>
   </si>
   <si>
-    <t>RAAS</t>
-  </si>
-  <si>
     <t>Enalapril</t>
   </si>
   <si>
     <t>Collagenase</t>
   </si>
   <si>
-    <t>ECM</t>
-  </si>
-  <si>
     <t>Skin</t>
   </si>
   <si>
@@ -137,9 +128,6 @@
     <t>PRM-151</t>
   </si>
   <si>
-    <t>GF Modulator</t>
-  </si>
-  <si>
     <t>Pamrevlumab</t>
   </si>
   <si>
@@ -152,10 +140,22 @@
     <t>Pirfenidone</t>
   </si>
   <si>
-    <t>IC Enz Inhibitor</t>
-  </si>
-  <si>
     <t>Anti-Inflammatory</t>
+  </si>
+  <si>
+    <t>HMGCoA inhibitor</t>
+  </si>
+  <si>
+    <t>RAAS inhibitor</t>
+  </si>
+  <si>
+    <t>ECM modulator</t>
+  </si>
+  <si>
+    <t>Intracellular Enzyme Inhibitor</t>
+  </si>
+  <si>
+    <t>Growth Factor Modulator</t>
   </si>
 </sst>
 </file>
@@ -510,7 +510,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:B21"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -622,10 +622,10 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
         <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
       </c>
       <c r="D8">
         <v>4</v>
@@ -633,10 +633,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -647,10 +647,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -661,13 +661,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11">
         <v>3</v>
@@ -675,13 +675,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D12">
         <v>4</v>
@@ -689,7 +689,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
         <v>38</v>
@@ -703,7 +703,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
         <v>38</v>
@@ -717,7 +717,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
         <v>38</v>
@@ -731,7 +731,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
         <v>38</v>
@@ -745,7 +745,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
         <v>38</v>
@@ -759,10 +759,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
@@ -773,10 +773,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
@@ -787,10 +787,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
@@ -801,10 +801,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
@@ -815,10 +815,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
@@ -829,10 +829,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C23" t="s">
         <v>6</v>
@@ -843,13 +843,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C24" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D24">
         <v>2</v>
@@ -857,13 +857,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C25" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D25">
         <v>2</v>
@@ -871,10 +871,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B26" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C26" t="s">
         <v>6</v>

</xml_diff>